<commit_message>
fixed drifting embers, added test with storage cleanup
</commit_message>
<xml_diff>
--- a/DownloadData_Performer/Data/Config.xlsx
+++ b/DownloadData_Performer/Data/Config.xlsx
@@ -10,8 +10,8 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="CYaDir8i9+9aXGt1T6W1O+TwC588l6bVVnVmd2bQY+M="/>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjft5lXGGzJXNnjsJNB79Vrrp5Pug=="/>
     </ext>
   </extLst>
 </workbook>
@@ -195,7 +195,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,13 +217,13 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -508,7 +507,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1583,10 +1582,10 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>0.0</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1594,11 +1593,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="5">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>16</v>
@@ -1606,112 +1605,112 @@
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>2.0</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <v>2.0</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1"/>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="5" t="b">
+      <c r="B17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="4" t="s">

</xml_diff>